<commit_message>
merge fig3 and fig4
</commit_message>
<xml_diff>
--- a/Data/Pertussis incidence.xlsx
+++ b/Data/Pertussis incidence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://6kmwxn-my.sharepoint.com/personal/kanggle_lkg1116_onmicrosoft_com/Documents/XMU/likangguo/2024/06 pertussis/WC_global/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://6kmwxn-my.sharepoint.com/personal/kanggle_lkg1116_onmicrosoft_com/Documents/XMU/likangguo/2024/06 pertussis/PertussisVaccine/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="88" documentId="11_199E324EA6E1A9EB1F2A0D0F8C40F4B9346263A5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1CCB04A0-540B-4A1A-A9AB-320913266994}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4014,10 +4014,10 @@
   <dimension ref="A1:AA223"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E127" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A187" sqref="A187"/>
+      <selection pane="bottomRight" activeCell="A157" sqref="A157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>